<commit_message>
Added Extent Reports & Uploaded a file
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Chamarie\IndustryConnect\onboardingSolution2\marsframework\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Chamarie\IndustryConnect\MarsCompetitionTask\MarsCompetitionTask\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6598E7-7E37-47A7-A815-24D2C225F9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D3CE3C-05BC-4E10-8394-A90141353688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13530" yWindow="555" windowWidth="11850" windowHeight="14805" activeTab="2" xr2:uid="{747B3E6C-4BEF-4585-9367-42A3372DE06D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{747B3E6C-4BEF-4585-9367-42A3372DE06D}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2185C4-0C52-4A19-8F20-94594A8B0317}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>